<commit_message>
#21 Enroll form updated person-create removed, person-edit updated scheduled_msgs form, task, tests and schedules removed Test added for enrollment
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/contact/person-edit.xlsx
+++ b/zazic-scale-up/forms/contact/person-edit.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech-21\zazic-scale-up\forms\contact\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865B067B-90AB-44B9-B66A-44F0E3230CCD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="survey" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="choices" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="settings" sheetId="3" r:id="rId6"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mjr6ItUWDb/UQJ1DfGI52oM1AUJXA=="/>
@@ -18,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="90">
   <si>
     <t>type</t>
   </si>
@@ -164,15 +173,6 @@
     <t>Zengeza Clinic</t>
   </si>
   <si>
-    <t>select_one facilities</t>
-  </si>
-  <si>
-    <t>enrollment_facility</t>
-  </si>
-  <si>
-    <t>VMMC Enrollment Facility</t>
-  </si>
-  <si>
     <t>enrollment_location</t>
   </si>
   <si>
@@ -294,77 +294,79 @@
   </si>
   <si>
     <t>Mahusekwa Hospital</t>
+  </si>
+  <si>
+    <t>NO_LABEL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Proxima Nova"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="10.0"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Proxima Nova"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12"/>
       <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -372,7 +374,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -381,8 +383,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FFD0CECE"/>
@@ -396,105 +404,55 @@
       <bottom style="thin">
         <color rgb="FFD0CECE"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -684,62 +642,62 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.11"/>
-    <col customWidth="1" min="2" max="2" width="18.44"/>
-    <col customWidth="1" min="3" max="3" width="57.0"/>
-    <col customWidth="1" min="4" max="4" width="11.33"/>
-    <col customWidth="1" min="5" max="5" width="4.0"/>
-    <col customWidth="1" min="6" max="8" width="13.44"/>
-    <col customWidth="1" min="9" max="9" width="64.0"/>
-    <col customWidth="1" min="10" max="18" width="13.44"/>
-    <col customWidth="1" min="19" max="26" width="10.0"/>
+    <col min="1" max="1" width="28.125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="57" customWidth="1"/>
+    <col min="4" max="4" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="64" customWidth="1"/>
+    <col min="10" max="18" width="13.5" customWidth="1"/>
+    <col min="19" max="26" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="15" t="s">
         <v>13</v>
       </c>
       <c r="K1" s="1"/>
@@ -759,23 +717,25 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -793,27 +753,27 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -831,29 +791,29 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -871,462 +831,454 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12" t="s">
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="C6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12" t="s">
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12" t="s">
+      <c r="B7" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="12" t="s">
+    <row r="8" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A8" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12" t="s">
+      <c r="B8" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
+    <row r="9" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A9" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
-      <c r="X9" s="12"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="12" t="s">
+    <row r="10" spans="1:26" ht="15.75">
+      <c r="A10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12" t="s">
+      <c r="C10" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
+      <c r="J11" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
+    <row r="12" spans="1:26" ht="15.75">
+      <c r="A12" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
+      <c r="B12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:26" ht="15.75">
+      <c r="A13" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14">
-      <c r="A14" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="12" t="s">
+    <row r="14" spans="1:26" ht="15.75">
+      <c r="A14" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15">
-      <c r="A15" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
+    <row r="15" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
+    <row r="16" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
+    <row r="17" spans="1:26" ht="15.75">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="16"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1349,17 +1301,17 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
+    <row r="18" spans="1:26" ht="15.75">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -1377,17 +1329,17 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
+    <row r="19" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -1405,8 +1357,8 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="16"/>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1433,7 +1385,7 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1461,17 +1413,17 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="18"/>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="16"/>
+      <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -1489,17 +1441,17 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="1"/>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="16"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -1517,17 +1469,17 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="16"/>
+    <row r="24" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A24" s="13"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="16"/>
+      <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -1545,41 +1497,14 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="16"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="12.75" customHeight="1"/>
-    <row r="29" ht="12.75" customHeight="1"/>
-    <row r="30" ht="12.75" customHeight="1"/>
-    <row r="31" ht="12.75" customHeight="1"/>
-    <row r="32" ht="12.75" customHeight="1"/>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:26" ht="12.75" customHeight="1"/>
+    <row r="28" spans="1:26" ht="12.75" customHeight="1"/>
+    <row r="29" spans="1:26" ht="12.75" customHeight="1"/>
+    <row r="30" spans="1:26" ht="12.75" customHeight="1"/>
+    <row r="31" spans="1:26" ht="12.75" customHeight="1"/>
+    <row r="32" spans="1:26" ht="12.75" customHeight="1"/>
     <row r="33" ht="12.75" customHeight="1"/>
     <row r="34" ht="12.75" customHeight="1"/>
     <row r="35" ht="12.75" customHeight="1"/>
@@ -1772,7 +1697,7 @@
     <row r="222" ht="12.75" customHeight="1"/>
     <row r="223" ht="12.75" customHeight="1"/>
     <row r="224" ht="12.75" customHeight="1"/>
-    <row r="225" ht="12.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
     <row r="226" ht="15.75" customHeight="1"/>
     <row r="227" ht="15.75" customHeight="1"/>
     <row r="228" ht="15.75" customHeight="1"/>
@@ -2547,36 +2472,31 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z985"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.67"/>
-    <col customWidth="1" min="2" max="2" width="13.44"/>
-    <col customWidth="1" min="3" max="3" width="17.67"/>
-    <col customWidth="1" min="4" max="6" width="13.44"/>
-    <col customWidth="1" min="7" max="26" width="8.56"/>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="17.625" customWidth="1"/>
+    <col min="4" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2587,7 +2507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="15.75">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -2598,7 +2518,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" ht="15.75">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2609,348 +2529,348 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:26" ht="15.75">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
     </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:26" ht="15.75">
+      <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="9"/>
-      <c r="Z9" s="9"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="7" t="s">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
+      <c r="B11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="7" t="s">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
+      <c r="B12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="7" t="s">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
+      <c r="B13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="7" t="s">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9"/>
+      <c r="B14" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
-    </row>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -3921,84 +3841,80 @@
     <row r="984" ht="15.75" customHeight="1"/>
     <row r="985" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="38.67"/>
-    <col customWidth="1" min="2" max="2" width="53.33"/>
-    <col customWidth="1" min="3" max="3" width="40.0"/>
-    <col customWidth="1" min="4" max="4" width="25.0"/>
-    <col customWidth="1" min="5" max="15" width="13.44"/>
-    <col customWidth="1" min="16" max="26" width="8.56"/>
+    <col min="1" max="1" width="38.625" customWidth="1"/>
+    <col min="2" max="2" width="53.375" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="15" width="13.5" customWidth="1"/>
+    <col min="16" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.0" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" ht="18" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="11">
-        <v>43936.0</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="10">
+        <v>43936</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -4981,9 +4897,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
zazic-scale-up: re-add enrollment facility question.
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/contact/person-edit.xlsx
+++ b/zazic-scale-up/forms/contact/person-edit.xlsx
@@ -1,76 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech-21\zazic-scale-up\forms\contact\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865B067B-90AB-44B9-B66A-44F0E3230CCD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" r:id="rId1"/>
-    <sheet name="choices" sheetId="2" r:id="rId2"/>
-    <sheet name="settings" sheetId="3" r:id="rId3"/>
+    <sheet state="visible" name="survey" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="choices" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="settings" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mjr6ItUWDb/UQJ1DfGI52oM1AUJXA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mhxE50lmiDDikQ5XQnYgO6cH2UVdw=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="93">
   <si>
     <t>type</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>relevant</t>
+  </si>
+  <si>
+    <t>appearance</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>hint</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>constraint_message</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
     <t>form_title</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>relevant</t>
-  </si>
-  <si>
-    <t>appearance</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>hint</t>
+    <t>begin group</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>NO_LABEL</t>
+  </si>
+  <si>
+    <t>field-list</t>
   </si>
   <si>
     <t>language_preference</t>
   </si>
   <si>
-    <t>default</t>
-  </si>
-  <si>
     <t>english</t>
   </si>
   <si>
-    <t>constraint</t>
-  </si>
-  <si>
-    <t>constraint_message</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -83,64 +86,100 @@
     <t>facilities</t>
   </si>
   <si>
-    <t>begin group</t>
-  </si>
-  <si>
-    <t>person</t>
-  </si>
-  <si>
-    <t>field-list</t>
+    <t>string</t>
+  </si>
+  <si>
+    <t>seke_north</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>Chitungwiza-Seke North clinic</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>PARENT</t>
+  </si>
+  <si>
+    <t>Person Type</t>
   </si>
   <si>
     <t>form_id</t>
   </si>
   <si>
-    <t>seke_north</t>
+    <t>mandatory</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>Chitungwiza-Seke North clinic</t>
-  </si>
-  <si>
     <t>style</t>
   </si>
   <si>
     <t>path</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>Parent</t>
-  </si>
-  <si>
-    <t>hidden</t>
+    <t>VMMC Client Name</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>regex(., "^[a-zA-Z\'\s]+$")</t>
+  </si>
+  <si>
+    <t>Please type in name characters e.g letters and space.</t>
   </si>
   <si>
     <t>seke_south</t>
   </si>
   <si>
-    <t>PARENT</t>
+    <t>Chitungwiza-Seke South clinic</t>
   </si>
   <si>
     <t>Edit Person</t>
   </si>
   <si>
-    <t>Chitungwiza-Seke South clinic</t>
+    <t>city_med</t>
+  </si>
+  <si>
+    <t>City Med hospital</t>
+  </si>
+  <si>
+    <t>select_one facilities</t>
   </si>
   <si>
     <t>contact:person:edit</t>
   </si>
   <si>
-    <t>Person Type</t>
-  </si>
-  <si>
-    <t>mandatory</t>
+    <t>enrollment_facility</t>
+  </si>
+  <si>
+    <t>VMMC Enrollment Facility</t>
+  </si>
+  <si>
+    <t>zengeza</t>
+  </si>
+  <si>
+    <t>Zengeza Clinic</t>
+  </si>
+  <si>
+    <t>chitungwiza_central</t>
+  </si>
+  <si>
+    <t>enrollment_location</t>
+  </si>
+  <si>
+    <t>Chitungwiza Central Hospital</t>
+  </si>
+  <si>
+    <t>Specify Enrollment Location</t>
   </si>
   <si>
     <t>pages</t>
@@ -149,40 +188,10 @@
     <t>data</t>
   </si>
   <si>
-    <t>city_med</t>
-  </si>
-  <si>
-    <t>City Med hospital</t>
-  </si>
-  <si>
-    <t>VMMC Client Name</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>regex(., "^[a-zA-Z\'\s]+$")</t>
-  </si>
-  <si>
-    <t>Please type in name characters e.g letters and space.</t>
-  </si>
-  <si>
-    <t>zengeza</t>
-  </si>
-  <si>
-    <t>Zengeza Clinic</t>
-  </si>
-  <si>
-    <t>enrollment_location</t>
-  </si>
-  <si>
-    <t>Specify Enrollment Location</t>
-  </si>
-  <si>
-    <t>chitungwiza_central</t>
-  </si>
-  <si>
-    <t>Chitungwiza Central Hospital</t>
+    <t>vmmc_no</t>
+  </si>
+  <si>
+    <t>VMMC Client Number</t>
   </si>
   <si>
     <t>chegutu_norton</t>
@@ -191,12 +200,6 @@
     <t>Chegutu- Norton hospital</t>
   </si>
   <si>
-    <t>vmmc_no</t>
-  </si>
-  <si>
-    <t>VMMC Client Number</t>
-  </si>
-  <si>
     <t>regex(., '^[0-9]{5,9}$')</t>
   </si>
   <si>
@@ -209,12 +212,12 @@
     <t>age_years</t>
   </si>
   <si>
+    <t>VMMC Client Age in Years</t>
+  </si>
+  <si>
     <t>chegutu_district</t>
   </si>
   <si>
-    <t>VMMC Client Age in Years</t>
-  </si>
-  <si>
     <t>Chegutu District Hospital</t>
   </si>
   <si>
@@ -233,22 +236,28 @@
     <t>Enrollment Date</t>
   </si>
   <si>
+    <t>monera</t>
+  </si>
+  <si>
     <t>decimal-date-time(.) = floor(decimal-date-time(today()))</t>
   </si>
   <si>
     <t>Only today's date is allowed</t>
   </si>
   <si>
+    <t>Monera clinic(Norton Outreach)</t>
+  </si>
+  <si>
     <t>phone</t>
   </si>
   <si>
     <t>Client Mobile phone number</t>
   </si>
   <si>
-    <t>monera</t>
-  </si>
-  <si>
-    <t>Monera clinic(Norton Outreach)</t>
+    <t>marondera</t>
+  </si>
+  <si>
+    <t>Marondera District Hospital</t>
   </si>
   <si>
     <t>regex(., '^\+263[0-9]{9}$')</t>
@@ -263,15 +272,15 @@
     <t>Alternative/Next of Kin's Mobile Number</t>
   </si>
   <si>
+    <t>mahusekwa</t>
+  </si>
+  <si>
+    <t>Mahusekwa Hospital</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
-    <t>marondera</t>
-  </si>
-  <si>
-    <t>Marondera District Hospital</t>
-  </si>
-  <si>
     <t>select_one language_preference</t>
   </si>
   <si>
@@ -287,86 +296,66 @@
     <t>Name of enrollment nurse</t>
   </si>
   <si>
-    <t>mahusekwa</t>
-  </si>
-  <si>
     <t>end group</t>
-  </si>
-  <si>
-    <t>Mahusekwa Hospital</t>
-  </si>
-  <si>
-    <t>NO_LABEL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
-      <sz val="12"/>
+      <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Cambria"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FFFFFFFF"/>
       <name val="Proxima Nova"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="12.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="12.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12.0"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="12.0"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -374,7 +363,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -384,13 +373,7 @@
     </fill>
   </fills>
   <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FFD0CECE"/>
@@ -404,55 +387,60 @@
       <bottom style="thin">
         <color rgb="FFD0CECE"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+  <cellXfs count="14">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -642,583 +630,591 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z999"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="28.125" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="57" customWidth="1"/>
-    <col min="4" max="4" width="11.375" customWidth="1"/>
-    <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="6" max="8" width="13.5" customWidth="1"/>
-    <col min="9" max="9" width="64" customWidth="1"/>
-    <col min="10" max="18" width="13.5" customWidth="1"/>
-    <col min="19" max="26" width="10" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="28.11"/>
+    <col customWidth="1" min="2" max="2" width="18.44"/>
+    <col customWidth="1" min="3" max="3" width="57.0"/>
+    <col customWidth="1" min="4" max="4" width="11.33"/>
+    <col customWidth="1" min="5" max="5" width="4.0"/>
+    <col customWidth="1" min="6" max="8" width="13.44"/>
+    <col customWidth="1" min="9" max="9" width="64.0"/>
+    <col customWidth="1" min="10" max="18" width="13.44"/>
+    <col customWidth="1" min="19" max="26" width="10.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A1" s="15" t="s">
+    <row r="1" ht="12.75" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
+    <row r="2" ht="12.75" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
+    <row r="3" ht="12.75" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A3" s="15" t="s">
+    <row r="4" ht="12.75" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="15" t="s">
+    <row r="5" ht="12.75" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
     </row>
-    <row r="5" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15" t="s">
+    <row r="6" ht="12.75" customHeight="1">
+      <c r="A6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-    </row>
-    <row r="6" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A6" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
+      <c r="B6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
       <c r="W6" s="11"/>
       <c r="X6" s="11"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A7" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15" t="s">
+    <row r="7" ht="12.75" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+    </row>
+    <row r="8" ht="12.75" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="C8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
     </row>
-    <row r="8" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A8" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15" t="s">
+    <row r="9" ht="12.75" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="C9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
     </row>
-    <row r="9" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A9" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="15" t="s">
+    <row r="10" ht="12.75" customHeight="1">
+      <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75">
-      <c r="A10" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
     </row>
-    <row r="11" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
+    <row r="12" ht="12.75" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75">
-      <c r="A12" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="15.75">
-      <c r="A13" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75">
-      <c r="A14" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-    </row>
-    <row r="15" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A15" s="1"/>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1228,283 +1224,310 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="12"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
+    <row r="16" ht="12.75" customHeight="1">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26" ht="15.75">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" ht="15.75">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
+    <row r="18">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
+    <row r="19">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
+    <row r="20" ht="12.75" customHeight="1">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A24" s="13"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:26" ht="12.75" customHeight="1"/>
-    <row r="28" spans="1:26" ht="12.75" customHeight="1"/>
-    <row r="29" spans="1:26" ht="12.75" customHeight="1"/>
-    <row r="30" spans="1:26" ht="12.75" customHeight="1"/>
-    <row r="31" spans="1:26" ht="12.75" customHeight="1"/>
-    <row r="32" spans="1:26" ht="12.75" customHeight="1"/>
+    <row r="25" ht="12.75" customHeight="1">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="12.75" customHeight="1"/>
+    <row r="29" ht="12.75" customHeight="1"/>
+    <row r="30" ht="12.75" customHeight="1"/>
+    <row r="31" ht="12.75" customHeight="1"/>
+    <row r="32" ht="12.75" customHeight="1"/>
     <row r="33" ht="12.75" customHeight="1"/>
     <row r="34" ht="12.75" customHeight="1"/>
     <row r="35" ht="12.75" customHeight="1"/>
@@ -1697,7 +1720,7 @@
     <row r="222" ht="12.75" customHeight="1"/>
     <row r="223" ht="12.75" customHeight="1"/>
     <row r="224" ht="12.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="225" ht="12.75" customHeight="1"/>
     <row r="226" ht="15.75" customHeight="1"/>
     <row r="227" ht="15.75" customHeight="1"/>
     <row r="228" ht="15.75" customHeight="1"/>
@@ -2472,405 +2495,410 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions/>
+  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z985"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
-    <col min="4" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="26" width="8.5" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="19.67"/>
+    <col customWidth="1" min="2" max="2" width="13.44"/>
+    <col customWidth="1" min="3" max="3" width="17.67"/>
+    <col customWidth="1" min="4" max="6" width="13.44"/>
+    <col customWidth="1" min="7" max="26" width="8.44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75">
-      <c r="A1" s="2" t="s">
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15.75">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    <row r="3">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75">
+    <row r="5">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
     </row>
-    <row r="6" spans="1:26" ht="15.75">
-      <c r="A6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="6" t="s">
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
+      <c r="C9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="8"/>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="6" t="s">
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
+      <c r="C12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="6" t="s">
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -3841,80 +3869,84 @@
     <row r="984" ht="15.75" customHeight="1"/>
     <row r="985" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
-    <col min="2" max="2" width="53.375" customWidth="1"/>
-    <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="15" width="13.5" customWidth="1"/>
-    <col min="16" max="26" width="8.5" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="38.67"/>
+    <col customWidth="1" min="2" max="2" width="53.33"/>
+    <col customWidth="1" min="3" max="3" width="40.0"/>
+    <col customWidth="1" min="4" max="4" width="25.0"/>
+    <col customWidth="1" min="5" max="15" width="13.44"/>
+    <col customWidth="1" min="16" max="26" width="8.44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" customHeight="1">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+    <row r="1" ht="18.0" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="10">
-        <v>43936</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="12">
+        <v>43936.0</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -4897,7 +4929,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
convert xlsx to xml
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/contact/person-edit.xlsx
+++ b/zazic-scale-up/forms/contact/person-edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuel-amodu/Desktop/medic-mobile/config-itech/zazic-scale-up/forms/contact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FA0326-221E-BC43-8E9F-0CD016469E90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDC7E96-BDFB-C64D-A040-388F460E76C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -709,9 +709,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -2576,9 +2576,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z984"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>